<commit_message>
work on analysis for apple
</commit_message>
<xml_diff>
--- a/output/Financial Statement AAPL/Compiled Balance Statement-AAPL.xlsx
+++ b/output/Financial Statement AAPL/Compiled Balance Statement-AAPL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliasusser/Desktop/Financial-Statements/output/Financial Statement AAPL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliasusser/Desktop/Financial-Statements /output/Financial Statement AAPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4849433F-A4FF-2E43-A8C6-B75933BC9844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1969A69F-CA86-2C4D-881A-CD9360183490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="500" windowWidth="22580" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled Statement" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="77">
   <si>
     <t>label</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>total liabilities and shareholders’ equity</t>
+  </si>
+  <si>
+    <t>long term debt</t>
+  </si>
+  <si>
+    <t>current term debt</t>
   </si>
 </sst>
 </file>
@@ -624,10 +630,10 @@
   <dimension ref="A1:AC46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2224,7 +2230,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B26">
         <v>3499</v>
@@ -2538,7 +2544,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B33">
         <v>73557</v>
@@ -2719,115 +2725,115 @@
         <v>65</v>
       </c>
       <c r="B35">
-        <f>SUM(B32:B34)</f>
+        <f t="shared" ref="B35:AC35" si="7">SUM(B32:B34)</f>
         <v>114621</v>
       </c>
       <c r="C35">
-        <f>SUM(C32:C34)</f>
+        <f t="shared" si="7"/>
         <v>127108</v>
       </c>
       <c r="D35">
-        <f>SUM(D32:D34)</f>
+        <f t="shared" si="7"/>
         <v>131446</v>
       </c>
       <c r="E35">
-        <f>SUM(E32:E34)</f>
+        <f t="shared" si="7"/>
         <v>140458</v>
       </c>
       <c r="F35">
-        <f>SUM(F32:F34)</f>
+        <f t="shared" si="7"/>
         <v>140458</v>
       </c>
       <c r="G35">
-        <f>SUM(G32:G34)</f>
+        <f t="shared" si="7"/>
         <v>150807</v>
       </c>
       <c r="H35">
-        <f>SUM(H32:H34)</f>
+        <f t="shared" si="7"/>
         <v>151304</v>
       </c>
       <c r="I35">
-        <f>SUM(I32:I34)</f>
+        <f t="shared" si="7"/>
         <v>145700</v>
       </c>
       <c r="J35">
-        <f>SUM(J32:J34)</f>
+        <f t="shared" si="7"/>
         <v>141712</v>
       </c>
       <c r="K35">
-        <f>SUM(K32:K34)</f>
+        <f t="shared" si="7"/>
         <v>141712</v>
       </c>
       <c r="L35">
-        <f>SUM(L32:L34)</f>
+        <f t="shared" si="7"/>
         <v>147544</v>
       </c>
       <c r="M35">
-        <f>SUM(M32:M34)</f>
+        <f t="shared" si="7"/>
         <v>142366</v>
       </c>
       <c r="N35">
-        <f>SUM(N32:N34)</f>
+        <f t="shared" si="7"/>
         <v>136079</v>
       </c>
       <c r="O35">
-        <f>SUM(O32:O34)</f>
+        <f t="shared" si="7"/>
         <v>142310</v>
       </c>
       <c r="P35">
-        <f>SUM(P32:P34)</f>
+        <f t="shared" si="7"/>
         <v>142310</v>
       </c>
       <c r="Q35">
-        <f>SUM(Q32:Q34)</f>
+        <f t="shared" si="7"/>
         <v>148926</v>
       </c>
       <c r="R35">
-        <f>SUM(R32:R34)</f>
+        <f t="shared" si="7"/>
         <v>145881</v>
       </c>
       <c r="S35">
-        <f>SUM(S32:S34)</f>
+        <f t="shared" si="7"/>
         <v>149744</v>
       </c>
       <c r="T35">
-        <f>SUM(T32:T34)</f>
+        <f t="shared" si="7"/>
         <v>153157</v>
       </c>
       <c r="U35">
-        <f>SUM(U32:U34)</f>
+        <f t="shared" si="7"/>
         <v>153157</v>
       </c>
       <c r="V35">
-        <f>SUM(V32:V34)</f>
+        <f t="shared" si="7"/>
         <v>155323</v>
       </c>
       <c r="W35">
-        <f>SUM(W32:W34)</f>
+        <f t="shared" si="7"/>
         <v>161595</v>
       </c>
       <c r="X35">
-        <f>SUM(X32:X34)</f>
+        <f t="shared" si="7"/>
         <v>157806</v>
       </c>
       <c r="Y35">
-        <f>SUM(Y32:Y34)</f>
+        <f t="shared" si="7"/>
         <v>162431</v>
       </c>
       <c r="Z35">
-        <f>SUM(Z32:Z34)</f>
+        <f t="shared" si="7"/>
         <v>162431</v>
       </c>
       <c r="AA35">
-        <f>SUM(AA32:AA34)</f>
+        <f t="shared" si="7"/>
         <v>161685</v>
       </c>
       <c r="AB35">
-        <f>SUM(AB32:AB34)</f>
+        <f t="shared" si="7"/>
         <v>155755</v>
       </c>
       <c r="AC35">
-        <f>SUM(AC32:AC34)</f>
+        <f t="shared" si="7"/>
         <v>148329</v>
       </c>
     </row>
@@ -2836,115 +2842,115 @@
         <v>66</v>
       </c>
       <c r="B38">
-        <f>B28+B35</f>
+        <f t="shared" ref="B38:AC38" si="8">B28+B35</f>
         <v>198751</v>
       </c>
       <c r="C38">
-        <f>C28+C35</f>
+        <f t="shared" si="8"/>
         <v>200450</v>
       </c>
       <c r="D38">
-        <f>D28+D35</f>
+        <f t="shared" si="8"/>
         <v>212748</v>
       </c>
       <c r="E38">
-        <f>E28+E35</f>
+        <f t="shared" si="8"/>
         <v>241272</v>
       </c>
       <c r="F38">
-        <f>F28+F35</f>
+        <f t="shared" si="8"/>
         <v>241272</v>
       </c>
       <c r="G38">
-        <f>G28+G35</f>
+        <f t="shared" si="8"/>
         <v>266595</v>
       </c>
       <c r="H38">
-        <f>H28+H35</f>
+        <f t="shared" si="8"/>
         <v>240624</v>
       </c>
       <c r="I38">
-        <f>I28+I35</f>
+        <f t="shared" si="8"/>
         <v>234248</v>
       </c>
       <c r="J38">
-        <f>J28+J35</f>
+        <f t="shared" si="8"/>
         <v>258578</v>
       </c>
       <c r="K38">
-        <f>K28+K35</f>
+        <f t="shared" si="8"/>
         <v>258578</v>
       </c>
       <c r="L38">
-        <f>L28+L35</f>
+        <f t="shared" si="8"/>
         <v>255827</v>
       </c>
       <c r="M38">
-        <f>M28+M35</f>
+        <f t="shared" si="8"/>
         <v>236138</v>
       </c>
       <c r="N38">
-        <f>N28+N35</f>
+        <f t="shared" si="8"/>
         <v>225783</v>
       </c>
       <c r="O38">
-        <f>O28+O35</f>
+        <f t="shared" si="8"/>
         <v>248028</v>
       </c>
       <c r="P38">
-        <f>P28+P35</f>
+        <f t="shared" si="8"/>
         <v>248028</v>
       </c>
       <c r="Q38">
-        <f>Q28+Q35</f>
+        <f t="shared" si="8"/>
         <v>251087</v>
       </c>
       <c r="R38">
-        <f>R28+R35</f>
+        <f t="shared" si="8"/>
         <v>241975</v>
       </c>
       <c r="S38">
-        <f>S28+S35</f>
+        <f t="shared" si="8"/>
         <v>245062</v>
       </c>
       <c r="T38">
-        <f>T28+T35</f>
+        <f t="shared" si="8"/>
         <v>258549</v>
       </c>
       <c r="U38">
-        <f>U28+U35</f>
+        <f t="shared" si="8"/>
         <v>258549</v>
       </c>
       <c r="V38">
-        <f>V28+V35</f>
+        <f t="shared" si="8"/>
         <v>287830</v>
       </c>
       <c r="W38">
-        <f>W28+W35</f>
+        <f t="shared" si="8"/>
         <v>267980</v>
       </c>
       <c r="X38">
-        <f>X28+X35</f>
+        <f t="shared" si="8"/>
         <v>265560</v>
       </c>
       <c r="Y38">
-        <f>Y28+Y35</f>
+        <f t="shared" si="8"/>
         <v>287912</v>
       </c>
       <c r="Z38">
-        <f>Z28+Z35</f>
+        <f t="shared" si="8"/>
         <v>287912</v>
       </c>
       <c r="AA38">
-        <f>AA28+AA35</f>
+        <f t="shared" si="8"/>
         <v>309259</v>
       </c>
       <c r="AB38">
-        <f>AB28+AB35</f>
+        <f t="shared" si="8"/>
         <v>283263</v>
       </c>
       <c r="AC38">
-        <f>AC28+AC35</f>
+        <f t="shared" si="8"/>
         <v>278202</v>
       </c>
     </row>
@@ -3321,67 +3327,67 @@
         <v>132390</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:AB45" si="7">C19-C38</f>
+        <f t="shared" ref="C45:AB45" si="9">C19-C38</f>
         <v>134082</v>
       </c>
       <c r="D45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>132425</v>
       </c>
       <c r="E45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>134047</v>
       </c>
       <c r="F45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>134047</v>
       </c>
       <c r="G45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>140199</v>
       </c>
       <c r="H45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>126878</v>
       </c>
       <c r="I45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>114949</v>
       </c>
       <c r="J45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>107147</v>
       </c>
       <c r="K45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>107147</v>
       </c>
       <c r="L45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>117892</v>
       </c>
       <c r="M45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>105860</v>
       </c>
       <c r="N45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>96456</v>
       </c>
       <c r="O45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>90488</v>
       </c>
       <c r="P45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>90488</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>89531</v>
       </c>
       <c r="R45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>78425</v>
       </c>
       <c r="S45">
@@ -3389,39 +3395,39 @@
         <v>72282</v>
       </c>
       <c r="T45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>65339</v>
       </c>
       <c r="U45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>65339</v>
       </c>
       <c r="V45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>66224</v>
       </c>
       <c r="W45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>69178</v>
       </c>
       <c r="X45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>64280</v>
       </c>
       <c r="Y45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>63090</v>
       </c>
       <c r="Z45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>63090</v>
       </c>
       <c r="AA45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>71932</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>67399</v>
       </c>
       <c r="AC45">
@@ -3438,111 +3444,111 @@
         <v>331141</v>
       </c>
       <c r="C46">
-        <f t="shared" ref="C46:AC46" si="8">C38+C45</f>
+        <f t="shared" ref="C46:AC46" si="10">C38+C45</f>
         <v>334532</v>
       </c>
       <c r="D46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>345173</v>
       </c>
       <c r="E46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>375319</v>
       </c>
       <c r="F46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>375319</v>
       </c>
       <c r="G46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>406794</v>
       </c>
       <c r="H46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>367502</v>
       </c>
       <c r="I46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>349197</v>
       </c>
       <c r="J46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>365725</v>
       </c>
       <c r="K46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>365725</v>
       </c>
       <c r="L46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>373719</v>
       </c>
       <c r="M46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>341998</v>
       </c>
       <c r="N46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>322239</v>
       </c>
       <c r="O46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>338516</v>
       </c>
       <c r="P46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>338516</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>340618</v>
       </c>
       <c r="R46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>320400</v>
       </c>
       <c r="S46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>317344</v>
       </c>
       <c r="T46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>323888</v>
       </c>
       <c r="U46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>323888</v>
       </c>
       <c r="V46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>354054</v>
       </c>
       <c r="W46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>337158</v>
       </c>
       <c r="X46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>329840</v>
       </c>
       <c r="Y46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>351002</v>
       </c>
       <c r="Z46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>351002</v>
       </c>
       <c r="AA46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>381191</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>350662</v>
       </c>
       <c r="AC46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>336309</v>
       </c>
     </row>

</xml_diff>